<commit_message>
Proper sequencer (2 channels, can play chords)
</commit_message>
<xml_diff>
--- a/Data Planning.xlsx
+++ b/Data Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_files\midi-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A6638-6A5F-49A8-89F6-06FD08405414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77D1B77-4104-4EEE-8B03-0751820A5BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A615CB41-7C92-4274-80FA-733F7F45E3F1}"/>
+    <workbookView xWindow="3540" yWindow="990" windowWidth="22695" windowHeight="14010" xr2:uid="{A615CB41-7C92-4274-80FA-733F7F45E3F1}"/>
   </bookViews>
   <sheets>
     <sheet name="1k" sheetId="1" r:id="rId1"/>
@@ -167,19 +167,19 @@
     <t>Per coord selection (ex: for transpose, ...)</t>
   </si>
   <si>
-    <t>Per note selection (ex: for velocity, …)</t>
-  </si>
-  <si>
-    <t>Coord trig</t>
-  </si>
-  <si>
-    <t>Note trig</t>
-  </si>
-  <si>
-    <t>Bytes needed to trigger a single chord</t>
-  </si>
-  <si>
-    <t>Bytes needed to trigger a single note</t>
+    <t>Chord selection</t>
+  </si>
+  <si>
+    <t>Bytes needed to select a single chord</t>
+  </si>
+  <si>
+    <t>Notes selection</t>
+  </si>
+  <si>
+    <t>Bytes needed to select notes (within chord)</t>
+  </si>
+  <si>
+    <t>Per notes selection (ex: for velocity, …)</t>
   </si>
 </sst>
 </file>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796D6850-C300-4ACD-A0B9-4ED99E766924}">
   <dimension ref="A2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,14 +1002,14 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="19">
         <f>_xlfn.CEILING.MATH((LOG(B11, 2)+B14)/8,1)</f>
         <v>1</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1032,14 +1032,14 @@
         <v>9</v>
       </c>
       <c r="B17" s="12">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="18">
         <f>B17*B16*E15</f>
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>29</v>
@@ -1061,14 +1061,14 @@
         <v>21</v>
       </c>
       <c r="B20" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="21"/>
       <c r="G20" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,11 +1076,11 @@
         <v>46</v>
       </c>
       <c r="E21" s="19">
-        <f>_xlfn.CEILING.MATH((LOG(B10, 2)+B20)/8,1)</f>
+        <f>_xlfn.CEILING.MATH((B10+B20)/8,1)</f>
         <v>1</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,14 +1103,14 @@
         <v>9</v>
       </c>
       <c r="B23" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="18">
         <f>B23*B22*E21</f>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>29</v>
@@ -1121,8 +1121,8 @@
         <v>17</v>
       </c>
       <c r="E24" s="18">
-        <f>_xlfn.CEILING.MATH(B22/8,1)*B23</f>
-        <v>8</v>
+        <f>B22*B23</f>
+        <v>32</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>31</v>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="E25" s="18">
         <f>E24</f>
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>32</v>
@@ -1156,14 +1156,14 @@
         <v>25</v>
       </c>
       <c r="B28" s="12">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="E28" s="18">
         <f>B28</f>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>42</v>
@@ -1174,7 +1174,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E29" s="21"/>
       <c r="G29" s="17" t="s">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="E31" s="22">
         <f>E11+B29*(E17+E23+E24+E25)+E28</f>
-        <v>976</v>
+        <v>336</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>34</v>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="E32" s="19">
         <f>1024-E31</f>
-        <v>48</v>
+        <v>688</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Simple storage to EEPROM
</commit_message>
<xml_diff>
--- a/Data Planning.xlsx
+++ b/Data Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_files\midi-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77D1B77-4104-4EEE-8B03-0751820A5BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74386C43-BA35-4D2A-8B80-0B9C8D2812CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="990" windowWidth="22695" windowHeight="14010" xr2:uid="{A615CB41-7C92-4274-80FA-733F7F45E3F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A615CB41-7C92-4274-80FA-733F7F45E3F1}"/>
   </bookViews>
   <sheets>
     <sheet name="1k" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Note</t>
   </si>
@@ -86,12 +86,6 @@
     <t>↗</t>
   </si>
   <si>
-    <t>Trigs on</t>
-  </si>
-  <si>
-    <t>Trigs off</t>
-  </si>
-  <si>
     <t>Nb channels</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>Vector of trigs (notes on)</t>
   </si>
   <si>
-    <t>Vector of trigs (notes off)</t>
-  </si>
-  <si>
     <t>Number of MIDI channels to control</t>
   </si>
   <si>
@@ -180,6 +171,9 @@
   </si>
   <si>
     <t>Per notes selection (ex: for velocity, …)</t>
+  </si>
+  <si>
+    <t>Trigs</t>
   </si>
 </sst>
 </file>
@@ -811,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796D6850-C300-4ACD-A0B9-4ED99E766924}">
-  <dimension ref="A2:K32"/>
+  <dimension ref="A2:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +827,7 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>16</v>
@@ -921,10 +915,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -935,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -953,7 +947,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -971,7 +965,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -980,36 +974,36 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" s="21"/>
       <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="12">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" s="21"/>
       <c r="G14" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" s="19">
         <f>_xlfn.CEILING.MATH((LOG(B11, 2)+B14)/8,1)</f>
         <v>1</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1024,7 +1018,7 @@
       </c>
       <c r="E16" s="21"/>
       <c r="G16" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,7 +1036,7 @@
         <v>32</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1051,36 +1045,36 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E19" s="21"/>
       <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="12">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" s="21"/>
       <c r="G20" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E21" s="19">
         <f>_xlfn.CEILING.MATH((B10+B20)/8,1)</f>
         <v>1</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1095,7 +1089,7 @@
       </c>
       <c r="E22" s="21"/>
       <c r="G22" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,104 +1107,92 @@
         <v>32</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E24" s="18">
         <f>B22*B23</f>
         <v>32</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="18">
-        <f>E24</f>
-        <v>32</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>32</v>
-      </c>
+      <c r="E25" s="21"/>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E26" s="21"/>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="21"/>
-      <c r="G27" s="17"/>
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="12">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="18">
+        <f>B27</f>
+        <v>64</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="12">
+        <v>2</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="G28" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="21"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="22">
+        <f>E11+B28*(E17+E23+E24)+E27</f>
+        <v>272</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="12">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="18">
-        <f>B28</f>
-        <v>64</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="12">
-        <v>2</v>
-      </c>
-      <c r="E29" s="21"/>
-      <c r="G29" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="21"/>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="22">
-        <f>E11+B29*(E17+E23+E24+E25)+E28</f>
-        <v>336</v>
+      <c r="E31" s="19">
+        <f>1024-E30</f>
+        <v>752</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="19">
-        <f>1024-E31</f>
-        <v>688</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>